<commit_message>
update the delivery fee for fbe students
</commit_message>
<xml_diff>
--- a/weekly_summary.xlsx
+++ b/weekly_summary.xlsx
@@ -234,12 +234,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Weekly Summary'!$A$17:$A$20</f>
+              <f>'Weekly Summary'!$A$17:$A$22</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Weekly Summary'!$B$17:$B$20</f>
+              <f>'Weekly Summary'!$B$17:$B$22</f>
             </numRef>
           </val>
         </ser>
@@ -315,7 +315,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>21</row>
+      <row>23</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5040000" cy="2880000"/>
@@ -625,7 +625,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -635,17 +635,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="60" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="19" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
     <col width="9" customWidth="1" min="4" max="4"/>
     <col width="35" customWidth="1" min="5" max="5"/>
-    <col width="7" customWidth="1" min="6" max="6"/>
+    <col width="9" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1" ht="28" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>📊 Weekly Summary • Dec 21 → Dec 28, 2025</t>
+          <t>📊 Weekly Summary • Jan 01 → Jan 11, 2026</t>
         </is>
       </c>
     </row>
@@ -664,7 +664,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5">
@@ -674,7 +674,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6">
@@ -684,7 +684,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7"/>
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>9</v>
+        <v>186</v>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>147</v>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
@@ -718,7 +718,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>4</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10">
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="B10" s="4" t="n">
-        <v>11.1</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11"/>
@@ -746,7 +746,7 @@
         </is>
       </c>
       <c r="B13" s="5" t="n">
-        <v>120</v>
+        <v>28455</v>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>10</v>
+        <v>1980</v>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="F13" s="5" t="n">
-        <v>130</v>
+        <v>30435</v>
       </c>
     </row>
     <row r="14"/>
@@ -798,7 +798,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Abudabi #6kilo</t>
+          <t>ክርስቲና ምግብ ቤት</t>
         </is>
       </c>
       <c r="B17" s="5" t="n">
@@ -808,13 +808,13 @@
         <v>0</v>
       </c>
       <c r="D17" s="7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Tena Mgb Bet</t>
+          <t>Test Vendor</t>
         </is>
       </c>
       <c r="B18" s="5" t="n">
@@ -830,7 +830,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Abudabi #5kilo</t>
+          <t>መቅዲ ምግብ ቤት</t>
         </is>
       </c>
       <c r="B19" s="5" t="n">
@@ -846,130 +846,169 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Test Vendor</t>
+          <t>ቲጂ አቡዳቢ #5kilo</t>
         </is>
       </c>
       <c r="B20" s="5" t="n">
-        <v>120</v>
+        <v>12930</v>
       </c>
       <c r="C20" s="5" t="n">
-        <v>130</v>
+        <v>14060</v>
       </c>
       <c r="D20" s="7" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23">
-      <c r="A23" s="2" t="inlineStr">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>ቲጂ አቡዳቢ #6kilo</t>
+        </is>
+      </c>
+      <c r="B21" s="5" t="n">
+        <v>8680</v>
+      </c>
+      <c r="C21" s="5" t="n">
+        <v>9285</v>
+      </c>
+      <c r="D21" s="7" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>ጤና ምግብ ቤት</t>
+        </is>
+      </c>
+      <c r="B22" s="5" t="n">
+        <v>6845</v>
+      </c>
+      <c r="C22" s="5" t="n">
+        <v>7330</v>
+      </c>
+      <c r="D22" s="7" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
         <is>
           <t>🍜 TOP MEAL</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>ቴስቲ ወጥ ×5</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="3" t="inlineStr">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ሙሉ ኮርኒስ ×37</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="inlineStr">
         <is>
           <t>📍 TOP CAMPUS</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>6kilo (9 orders)</t>
-        </is>
-      </c>
-    </row>
-    <row r="25"/>
-    <row r="26">
-      <c r="A26" s="2" t="inlineStr">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>6kilo (84 orders)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27"/>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
         <is>
           <t>🛵 DELIVERY SQUAD</t>
         </is>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="6" t="inlineStr">
+    <row r="29">
+      <c r="A29" s="6" t="inlineStr">
         <is>
           <t>Active DGs</t>
         </is>
       </c>
-      <c r="B27" s="6" t="inlineStr">
+      <c r="B29" s="6" t="inlineStr">
         <is>
           <t>Total Deliveries</t>
         </is>
       </c>
-      <c r="C27" s="6" t="inlineStr">
+      <c r="C29" s="6" t="inlineStr">
         <is>
           <t>Acceptance Rate</t>
         </is>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>1</v>
-      </c>
-      <c r="B28" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" s="4" t="n">
+    <row r="30">
+      <c r="A30" t="n">
+        <v>2</v>
+      </c>
+      <c r="B30" t="n">
+        <v>15</v>
+      </c>
+      <c r="C30" s="4" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="29"/>
-    <row r="30">
-      <c r="A30" s="2" t="inlineStr">
+    <row r="31"/>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
         <is>
           <t>❌ CANCELLATIONS (sample)</t>
         </is>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
+    <row r="33">
+      <c r="A33" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
     </row>
-    <row r="32"/>
-    <row r="33">
-      <c r="A33" s="2" t="inlineStr">
+    <row r="34"/>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr">
         <is>
           <t>🧠 RECOMMENDATIONS</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>High cancellation rate this week (44.4%). Investigate top cancelled meals/vendors and contact them.</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Vendors with low reliability: Abudabi #6kilo, Tena Mgb Bet, Abudabi #5kilo. Consider warnings, training, or temporary delisting.</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>High cancellation rate this week (20.4%). Investigate top cancelled meals/vendors and contact them.</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Vendors with low reliability: ክርስቲና ምግብ ቤት, Test Vendor, መቅዲ ምግብ ቤት. Consider warnings, training, or temporary delisting.</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
           <t>DG acceptance low (0.0%). Consider incentives during peaks or recruit more DGs.</t>
         </is>
       </c>
     </row>
-    <row r="37"/>
-    <row r="38">
-      <c r="E38" s="8" t="inlineStr">
-        <is>
-          <t>Prepared on: 2025-12-28 20:47 UTC</t>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Top canceller: ቲጂ አቡዳቢ #5kilo with 15 cancels. Investigate immediately.</t>
+        </is>
+      </c>
+    </row>
+    <row r="40"/>
+    <row r="41">
+      <c r="E41" s="8" t="inlineStr">
+        <is>
+          <t>Prepared on: 2026-01-11 11:06 UTC</t>
         </is>
       </c>
     </row>

</xml_diff>